<commit_message>
Added working code in "TestClass"
</commit_message>
<xml_diff>
--- a/Selenium/src/com/datadriven/test/TestData.xlsx
+++ b/Selenium/src/com/datadriven/test/TestData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pragya.sharma/eclipse-workspace/Selenium/src/com/datadriven/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pragya.sharma/git/TestAssignment/Selenium/src/com/datadriven/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E54779-BED9-F24E-8936-36EF1D3EDC29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D6263EB6-73A0-7F44-8095-F635AB171A52}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15960" xr2:uid="{45CF048A-74F5-6C4D-BCB6-EFB74B971F4D}"/>
+    <workbookView windowHeight="15960" windowWidth="28040" xWindow="380" xr2:uid="{7548C9DC-4B3F-2640-9184-6234ABE33C74}" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="ExcelData" sheetId="1" r:id="rId1"/>
+    <sheet name="ExcelData" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,97 +25,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>HotelName</t>
+  </si>
   <si>
     <t>Price</t>
   </si>
   <si>
-    <t>HotelName</t>
-  </si>
-  <si>
-    <t>Jade 735</t>
-  </si>
-  <si>
-    <t>Rs150,000</t>
-  </si>
-  <si>
-    <t>Taj Bangalore</t>
-  </si>
-  <si>
-    <t>Rs140,000</t>
-  </si>
-  <si>
-    <t>TRANQUIL WOODS BY JADE</t>
-  </si>
-  <si>
-    <t>Rs129,000</t>
-  </si>
-  <si>
-    <t>Lotus By Jade</t>
-  </si>
-  <si>
-    <t>Rs90,000</t>
-  </si>
-  <si>
-    <t>Shreyas Yoga Retreat, Bangalore</t>
-  </si>
-  <si>
-    <t>Rs72,960</t>
-  </si>
-  <si>
-    <t>Lantern By Jade</t>
-  </si>
-  <si>
-    <t>Rs71,000</t>
-  </si>
-  <si>
-    <t>FabExpress Move Inn</t>
-  </si>
-  <si>
-    <t>Rs54,000</t>
-  </si>
-  <si>
-    <t>Shangri-La Hotel Bengaluru</t>
-  </si>
-  <si>
-    <t>Rs41,750</t>
-  </si>
-  <si>
     <t>The Ritz-Carlton, Bangalore</t>
-  </si>
-  <si>
-    <t>Rs40,500</t>
-  </si>
-  <si>
-    <t>Capital O 30373 Himalaya By Monarch</t>
-  </si>
-  <si>
-    <t>Rs40,179</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,21 +67,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -169,10 +95,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -207,7 +133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -259,7 +185,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -370,21 +296,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -401,7 +327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -453,118 +379,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F705870E-29B8-554C-87E8-E4A77D869A8A}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0378E7A4-9E7A-E846-ADBA-F89243936545}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.1484375" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="12.1640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>